<commit_message>
cuadrados latinos - bloques -efectos fijos y aleatorios
</commit_message>
<xml_diff>
--- a/Semana 6/datos_anova.xlsx
+++ b/Semana 6/datos_anova.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrodriguez\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\GITHUB\DESIGN-OF-EXPERIMENTS\Semana 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC1BF50-022B-484C-9363-B2471E67AAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88840279-37FE-4FFC-8F38-703FFD6F2936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7380" yWindow="2220" windowWidth="21600" windowHeight="11385" xr2:uid="{EB47FBFA-F97B-41F2-8C7F-4D8A137023A2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{EB47FBFA-F97B-41F2-8C7F-4D8A137023A2}"/>
   </bookViews>
   <sheets>
     <sheet name="E0" sheetId="5" r:id="rId1"/>
@@ -134,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -151,6 +151,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -169,7 +172,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -487,13 +490,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76B7C34E-9CFE-4ECB-A5D4-7610484B5B73}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -510,7 +513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -527,7 +530,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -544,7 +547,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -561,7 +564,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -591,9 +594,9 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -610,7 +613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>23.46</v>
       </c>
@@ -627,7 +630,7 @@
         <v>23.29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>23.48</v>
       </c>
@@ -644,7 +647,7 @@
         <v>23.46</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>23.56</v>
       </c>
@@ -661,7 +664,7 @@
         <v>23.37</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>23.39</v>
       </c>
@@ -678,7 +681,7 @@
         <v>23.32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>23.4</v>
       </c>
@@ -708,12 +711,12 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -725,7 +728,7 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -746,7 +749,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -767,7 +770,7 @@
       </c>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -787,7 +790,7 @@
         <v>80.626000000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -823,12 +826,12 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -839,7 +842,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -856,7 +859,7 @@
         <v>2890</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -873,7 +876,7 @@
         <v>3150</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -890,7 +893,7 @@
         <v>3050</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -917,99 +920,111 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{193F7EF7-02BA-45BD-B343-56A721C58E9F}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="5"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" s="7"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>65</v>
       </c>
       <c r="B2" s="2">
-        <v>82</v>
-      </c>
-      <c r="C2" s="2">
         <v>64</v>
       </c>
-      <c r="D2" s="2">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>81</v>
       </c>
       <c r="B3" s="2">
-        <v>67</v>
-      </c>
-      <c r="C3" s="2">
         <v>71</v>
       </c>
-      <c r="D3" s="2">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>57</v>
       </c>
       <c r="B4" s="2">
-        <v>59</v>
-      </c>
-      <c r="C4" s="2">
         <v>83</v>
       </c>
-      <c r="D4" s="2">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>66</v>
       </c>
       <c r="B5" s="2">
-        <v>75</v>
-      </c>
-      <c r="C5" s="2">
         <v>59</v>
       </c>
-      <c r="D5" s="2">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>82</v>
       </c>
       <c r="B6" s="2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>82</v>
+      </c>
+      <c r="B7" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>67</v>
+      </c>
+      <c r="B8" s="2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>59</v>
+      </c>
+      <c r="B9" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>75</v>
+      </c>
+      <c r="B10" s="2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
         <v>70</v>
       </c>
-      <c r="C6" s="2">
-        <v>65</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="B11" s="2">
         <v>79</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>